<commit_message>
added additional gazeCal session for 3013
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B18BCA3-072F-8843-BFF2-B6C7008ABFEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB7238D-F6C1-9645-93C0-BF458014F3F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="800" windowWidth="24620" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="2700" yWindow="2400" windowWidth="24620" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eyeTrackingParams" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9800" uniqueCount="1267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9802" uniqueCount="1268">
   <si>
     <t>projectSubfolder</t>
   </si>
@@ -3831,16 +3831,19 @@
   </si>
   <si>
     <t>112816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 681, 835, 997, 1131, 1251, 1325, 1496, 1623, 1724 ] </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3886,6 +3889,7 @@
       <sz val="12"/>
       <color rgb="FF24292E"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3914,17 +3918,25 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Courier"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Helv"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3955,7 +3967,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4009,11 +4021,12 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -4353,17 +4366,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AP979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AF157" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AG77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AI160" sqref="AI160"/>
+      <selection pane="bottomRight" activeCell="AJ90" sqref="AJ90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7300,6 +7313,12 @@
       <c r="L90" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="AJ90" s="37" t="s">
+        <v>1267</v>
+      </c>
+      <c r="AK90" s="37" t="s">
+        <v>870</v>
+      </c>
     </row>
     <row r="92" spans="1:42">
       <c r="A92" s="4" t="s">

</xml_diff>

<commit_message>
Fixed glint mask for 3037 retino 4
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB7238D-F6C1-9645-93C0-BF458014F3F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C228BAF8-2DAF-D342-98AA-9B5454C79952}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="2400" windowWidth="24620" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="2140" windowWidth="24620" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eyeTrackingParams" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9802" uniqueCount="1268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9802" uniqueCount="1269">
   <si>
     <t>projectSubfolder</t>
   </si>
@@ -3834,6 +3834,9 @@
   </si>
   <si>
     <t xml:space="preserve">[ 681, 835, 997, 1131, 1251, 1325, 1496, 1623, 1724 ] </t>
+  </si>
+  <si>
+    <t>[148   244   253   215]</t>
   </si>
 </sst>
 </file>
@@ -4373,10 +4376,10 @@
   <dimension ref="A1:AP979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AG77" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E276" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ90" sqref="AJ90"/>
+      <selection pane="bottomRight" activeCell="E292" sqref="E292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13948,7 +13951,7 @@
         <v>32</v>
       </c>
       <c r="E292" s="4" t="s">
-        <v>795</v>
+        <v>1268</v>
       </c>
       <c r="F292" s="4" t="s">
         <v>629</v>

</xml_diff>

<commit_message>
Bug fix for 3040 params for missing gaze cal
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C228BAF8-2DAF-D342-98AA-9B5454C79952}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD05FEF-F2FA-F44D-AB10-9EB8FF1DFCF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="2140" windowWidth="24620" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="920" windowWidth="24620" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eyeTrackingParams" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -4376,10 +4376,10 @@
   <dimension ref="A1:AP979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E276" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AI894" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E292" sqref="E292"/>
+      <selection pane="bottomRight" activeCell="AL909" sqref="AL909"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -34525,7 +34525,7 @@
         <v>1087</v>
       </c>
       <c r="AM905" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="AN905" t="s">
         <v>1059</v>
@@ -34790,8 +34790,8 @@
       <c r="X912" s="5" t="s">
         <v>1087</v>
       </c>
-      <c r="AM912" s="5" t="s">
-        <v>1100</v>
+      <c r="AM912" t="s">
+        <v>1099</v>
       </c>
       <c r="AN912" t="s">
         <v>1059</v>
@@ -34828,8 +34828,8 @@
       <c r="X913" s="5" t="s">
         <v>1087</v>
       </c>
-      <c r="AM913" s="5" t="s">
-        <v>1100</v>
+      <c r="AM913" t="s">
+        <v>1099</v>
       </c>
       <c r="AN913" t="s">
         <v>1059</v>

</xml_diff>

<commit_message>
Bad frame specification for 3037 sess 1
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FB998B-1D89-5D4E-8BAF-716089CE3809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7B7AAE-C3BC-204D-9D74-E36491F239BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="920" windowWidth="24620" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3818,9 +3818,6 @@
     <t>[136, 558, 2640, 3755, 4894, 5211, 7824. 9464, 11293, 12559, 13220, 14370, 15570, 17328, 19083]</t>
   </si>
   <si>
-    <t>[11, 766, 1586, 3125, 4268, 5459, 6796, 8709, 9790, 105881, 11550, 12781, 14093, 17111, 19348]</t>
-  </si>
-  <si>
     <t>[466, 1180, 1889, 3037, 4004, 5391, 6321, 7584, 8547, 9842, 11124, 12377, 13421, 17097, 19010]</t>
   </si>
   <si>
@@ -3843,6 +3840,9 @@
   </si>
   <si>
     <t>[-0.50; 5.50]</t>
+  </si>
+  <si>
+    <t>[11, 766, 1586, 3125, 4268, 5459, 6796, 8709, 9790, 11550, 12781, 14093, 17111, 19348]</t>
   </si>
 </sst>
 </file>
@@ -4382,10 +4382,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AI582" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AI280" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AM592" sqref="AM592"/>
+      <selection pane="bottomRight" activeCell="AJ290" sqref="AJ290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4535,7 +4535,7 @@
         <v>1102</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>272</v>
@@ -7289,7 +7289,7 @@
         <v>100</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="AD89" s="13">
         <v>27.49</v>
@@ -7309,7 +7309,7 @@
         <v>100</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>95</v>
@@ -7327,7 +7327,7 @@
         <v>58</v>
       </c>
       <c r="AJ90" s="37" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="AK90" s="37" t="s">
         <v>870</v>
@@ -13876,7 +13876,7 @@
         <v>805</v>
       </c>
       <c r="AJ290" t="s">
-        <v>1262</v>
+        <v>1270</v>
       </c>
       <c r="AN290" s="5" t="s">
         <v>95</v>
@@ -13938,7 +13938,7 @@
         <v>805</v>
       </c>
       <c r="AJ291" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="AN291" s="5" t="s">
         <v>95</v>
@@ -13961,7 +13961,7 @@
         <v>32</v>
       </c>
       <c r="E292" s="4" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="F292" s="4" t="s">
         <v>629</v>
@@ -14000,7 +14000,7 @@
         <v>805</v>
       </c>
       <c r="AJ292" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="AN292" s="5" t="s">
         <v>95</v>
@@ -23502,7 +23502,7 @@
       </c>
       <c r="AD589" s="15"/>
       <c r="AJ589" s="5" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="AK589" s="5" t="s">
         <v>1049</v>
@@ -23603,7 +23603,7 @@
         <v>1087</v>
       </c>
       <c r="AM591" s="5" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="AN591" t="s">
         <v>1098</v>

</xml_diff>

<commit_message>
x0 cameraTrans for several sceneSync cases
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7B7AAE-C3BC-204D-9D74-E36491F239BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F56F07-99AA-B34E-A728-32CE1646AC35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="920" windowWidth="24620" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5980" yWindow="2360" windowWidth="21780" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eyeTrackingParams" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9804" uniqueCount="1271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9832" uniqueCount="1299">
   <si>
     <t>projectSubfolder</t>
   </si>
@@ -3843,6 +3843,90 @@
   </si>
   <si>
     <t>[11, 766, 1586, 3125, 4268, 5459, 6796, 8709, 9790, 11550, 12781, 14093, 17111, 19348]</t>
+  </si>
+  <si>
+    <t>[-3.83; 1.26]</t>
+  </si>
+  <si>
+    <t>[2.44; -2.81]</t>
+  </si>
+  <si>
+    <t>[2.69; -3.20]</t>
+  </si>
+  <si>
+    <t>[3.33; -2.20]</t>
+  </si>
+  <si>
+    <t>[0.00; -5.97]</t>
+  </si>
+  <si>
+    <t>[4.74; -3.50]</t>
+  </si>
+  <si>
+    <t>[-1.50; 2.02]</t>
+  </si>
+  <si>
+    <t>[0.12; 3.91]</t>
+  </si>
+  <si>
+    <t>[-2.50; -2.21]</t>
+  </si>
+  <si>
+    <t>[-2.50; -2.48]</t>
+  </si>
+  <si>
+    <t>[0.30; 2.13]</t>
+  </si>
+  <si>
+    <t>[0.22; 0.90]</t>
+  </si>
+  <si>
+    <t>[0.05; -2.64]</t>
+  </si>
+  <si>
+    <t>[1.30; 0.50]</t>
+  </si>
+  <si>
+    <t>[0.00; -2.21]</t>
+  </si>
+  <si>
+    <t>[0.00; -2.30]</t>
+  </si>
+  <si>
+    <t>[-1.00; 1.63]</t>
+  </si>
+  <si>
+    <t>[-2.50; 1.57]</t>
+  </si>
+  <si>
+    <t>[-2.00; -0.80]</t>
+  </si>
+  <si>
+    <t>[-1.50; 0.83]</t>
+  </si>
+  <si>
+    <t>[-0.62; 1.15]</t>
+  </si>
+  <si>
+    <t>[0.00; 4.78]</t>
+  </si>
+  <si>
+    <t>[0.40; 4.54]</t>
+  </si>
+  <si>
+    <t>[0.50; 1.02]</t>
+  </si>
+  <si>
+    <t>[1.50; 3.67]</t>
+  </si>
+  <si>
+    <t>[2.00; 6.02]</t>
+  </si>
+  <si>
+    <t>[-1.00; 1.90]</t>
+  </si>
+  <si>
+    <t>[-3.77; 2.33]</t>
   </si>
 </sst>
 </file>
@@ -4382,10 +4466,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AI280" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AL888" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ290" sqref="AJ290"/>
+      <selection pane="bottomRight" activeCell="AM882" sqref="AM882"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5533,6 +5617,9 @@
       <c r="X32" s="5" t="s">
         <v>738</v>
       </c>
+      <c r="AM32" s="5" t="s">
+        <v>1271</v>
+      </c>
       <c r="AN32" s="5" t="s">
         <v>95</v>
       </c>
@@ -5960,6 +6047,9 @@
       <c r="AJ45" s="5" t="s">
         <v>1243</v>
       </c>
+      <c r="AM45" t="s">
+        <v>1272</v>
+      </c>
       <c r="AN45" s="5" t="s">
         <v>95</v>
       </c>
@@ -6016,6 +6106,9 @@
       <c r="AJ46" s="5" t="s">
         <v>1244</v>
       </c>
+      <c r="AM46" t="s">
+        <v>1273</v>
+      </c>
       <c r="AN46" s="5" t="s">
         <v>95</v>
       </c>
@@ -6913,6 +7006,9 @@
       <c r="X75" s="5" t="s">
         <v>727</v>
       </c>
+      <c r="AM75" t="s">
+        <v>1274</v>
+      </c>
       <c r="AN75" s="5" t="s">
         <v>1105</v>
       </c>
@@ -11186,6 +11282,9 @@
       <c r="X211" s="5" t="s">
         <v>727</v>
       </c>
+      <c r="AM211" s="5" t="s">
+        <v>1275</v>
+      </c>
       <c r="AN211" s="5" t="s">
         <v>95</v>
       </c>
@@ -11732,6 +11831,9 @@
       <c r="X226" s="5" t="s">
         <v>727</v>
       </c>
+      <c r="AM226" s="5" t="s">
+        <v>1276</v>
+      </c>
       <c r="AN226" s="5" t="s">
         <v>95</v>
       </c>
@@ -11922,6 +12024,9 @@
       <c r="X233" s="5" t="s">
         <v>727</v>
       </c>
+      <c r="AM233" s="5" t="s">
+        <v>1277</v>
+      </c>
       <c r="AN233" s="5" t="s">
         <v>95</v>
       </c>
@@ -12080,6 +12185,9 @@
       </c>
       <c r="X236" s="5" t="s">
         <v>728</v>
+      </c>
+      <c r="AM236" t="s">
+        <v>1278</v>
       </c>
       <c r="AN236" s="5" t="s">
         <v>95</v>
@@ -17542,6 +17650,9 @@
       <c r="X402" s="5" t="s">
         <v>1087</v>
       </c>
+      <c r="AM402" t="s">
+        <v>1279</v>
+      </c>
       <c r="AN402" s="5" t="s">
         <v>1098</v>
       </c>
@@ -18285,6 +18396,9 @@
       </c>
       <c r="X425" s="5" t="s">
         <v>1087</v>
+      </c>
+      <c r="AM425" s="5" t="s">
+        <v>1280</v>
       </c>
       <c r="AN425" t="s">
         <v>1101</v>
@@ -19415,6 +19529,9 @@
       <c r="X457" s="5" t="s">
         <v>1087</v>
       </c>
+      <c r="AM457" s="5" t="s">
+        <v>1281</v>
+      </c>
       <c r="AN457" t="s">
         <v>1101</v>
       </c>
@@ -19555,6 +19672,9 @@
       <c r="X461" s="5" t="s">
         <v>1087</v>
       </c>
+      <c r="AM461" s="5" t="s">
+        <v>1282</v>
+      </c>
       <c r="AN461" t="s">
         <v>1101</v>
       </c>
@@ -19660,6 +19780,9 @@
       <c r="X464" s="5" t="s">
         <v>1087</v>
       </c>
+      <c r="AM464" t="s">
+        <v>1283</v>
+      </c>
       <c r="AN464" s="5" t="s">
         <v>1101</v>
       </c>
@@ -19694,6 +19817,9 @@
       </c>
       <c r="X465" s="5" t="s">
         <v>1087</v>
+      </c>
+      <c r="AM465" t="s">
+        <v>1284</v>
       </c>
       <c r="AN465" s="5" t="s">
         <v>1101</v>
@@ -21309,6 +21435,9 @@
       <c r="AA518" s="5">
         <v>400</v>
       </c>
+      <c r="AM518" t="s">
+        <v>1285</v>
+      </c>
       <c r="AN518" t="s">
         <v>1101</v>
       </c>
@@ -21537,6 +21666,9 @@
       </c>
       <c r="X523" s="5" t="s">
         <v>1087</v>
+      </c>
+      <c r="AM523" s="5" t="s">
+        <v>1286</v>
       </c>
       <c r="AN523" s="5" t="s">
         <v>1101</v>
@@ -21828,6 +21960,9 @@
       <c r="X534" s="5" t="s">
         <v>1087</v>
       </c>
+      <c r="AM534" s="5" t="s">
+        <v>1287</v>
+      </c>
       <c r="AN534" t="s">
         <v>1098</v>
       </c>
@@ -21914,6 +22049,9 @@
       </c>
       <c r="X537" s="5" t="s">
         <v>1087</v>
+      </c>
+      <c r="AM537" s="5" t="s">
+        <v>1288</v>
       </c>
       <c r="AN537" s="5" t="s">
         <v>1098</v>
@@ -22752,6 +22890,9 @@
       <c r="X567" s="5" t="s">
         <v>1087</v>
       </c>
+      <c r="AM567" t="s">
+        <v>1289</v>
+      </c>
       <c r="AN567" s="5" t="s">
         <v>1099</v>
       </c>
@@ -22856,6 +22997,9 @@
       </c>
       <c r="X570" s="5" t="s">
         <v>1087</v>
+      </c>
+      <c r="AM570" t="s">
+        <v>1290</v>
       </c>
       <c r="AN570" s="5" t="s">
         <v>1100</v>
@@ -26185,6 +26329,9 @@
       <c r="X659" s="5" t="s">
         <v>1087</v>
       </c>
+      <c r="AM659" t="s">
+        <v>1291</v>
+      </c>
       <c r="AN659" t="s">
         <v>1098</v>
       </c>
@@ -29142,6 +29289,9 @@
         <v>1087</v>
       </c>
       <c r="AD747" s="18"/>
+      <c r="AM747" t="s">
+        <v>1292</v>
+      </c>
       <c r="AN747" t="s">
         <v>1099</v>
       </c>
@@ -29193,6 +29343,9 @@
         <v>1087</v>
       </c>
       <c r="AD748" s="18"/>
+      <c r="AM748" t="s">
+        <v>1293</v>
+      </c>
       <c r="AN748" t="s">
         <v>1099</v>
       </c>
@@ -31951,6 +32104,9 @@
       <c r="X832" s="5" t="s">
         <v>1087</v>
       </c>
+      <c r="AM832" t="s">
+        <v>1294</v>
+      </c>
       <c r="AN832" s="5" t="s">
         <v>1098</v>
       </c>
@@ -32513,6 +32669,9 @@
       <c r="X848" s="5" t="s">
         <v>1087</v>
       </c>
+      <c r="AM848" t="s">
+        <v>1295</v>
+      </c>
       <c r="AN848" s="5" t="s">
         <v>1099</v>
       </c>
@@ -32588,6 +32747,9 @@
       </c>
       <c r="X850" s="5" t="s">
         <v>1087</v>
+      </c>
+      <c r="AM850" t="s">
+        <v>1296</v>
       </c>
       <c r="AN850" s="5" t="s">
         <v>1098</v>
@@ -33463,6 +33625,9 @@
       <c r="X876" s="5" t="s">
         <v>1087</v>
       </c>
+      <c r="AM876" t="s">
+        <v>1297</v>
+      </c>
       <c r="AN876" t="s">
         <v>1099</v>
       </c>
@@ -33652,6 +33817,9 @@
       </c>
       <c r="X881" s="5" t="s">
         <v>1087</v>
+      </c>
+      <c r="AM881" s="5" t="s">
+        <v>1298</v>
       </c>
       <c r="AN881" s="5" t="s">
         <v>1099</v>

</xml_diff>

<commit_message>
Remove blank perimeter frame for 3019 sess 1 rest 4
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F56F07-99AA-B34E-A728-32CE1646AC35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DA8219-E214-3142-88BE-E0AC012625C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="2360" windowWidth="21780" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="1160" windowWidth="24420" windowHeight="15060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eyeTrackingParams" sheetId="1" r:id="rId1"/>
@@ -3767,9 +3767,6 @@
     <t>[1984, 8320, 13827, 17217, 17267, 18145]</t>
   </si>
   <si>
-    <t>[78, 158, 815, 1937, 3049, 4259, 5320, 6544, 7756, 9002, 10059, 11295, 12791, 14544, 17520]</t>
-  </si>
-  <si>
     <t>[5, 1004, 2084, 3289, 4608, 6030, 7051, 8119, 9517, 13357, 12656, 13912, 15454, 17830, 19249]</t>
   </si>
   <si>
@@ -3788,9 +3785,6 @@
     <t>[3, 837, 1754, 2823, 4000, 5174, 6190, 7540, 8623, 9707, 11258, 12566, 13628, 14910, 17672]</t>
   </si>
   <si>
-    <t>[4, 736, 1802, 2816, 3982, 5117, 6318, 8073, 9684, 11460, 12636, 13891, 15189, 16955, 18943]</t>
-  </si>
-  <si>
     <t>[5, 675, 1474, 2332, 3271, 4243, 5083, 6022, 7068, 7964, 8784, 9667, 10769, 14769, 17780]</t>
   </si>
   <si>
@@ -3927,6 +3921,12 @@
   </si>
   <si>
     <t>[-3.77; 2.33]</t>
+  </si>
+  <si>
+    <t>[158, 1937, 3049, 6544, 7756, 11295, 17520]</t>
+  </si>
+  <si>
+    <t>[4, 736, 1802, 2816, 5117, 6318, 8073, 9684, 11460, 12636, 13891, 15189, 16955, 18943]</t>
   </si>
 </sst>
 </file>
@@ -4466,10 +4466,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AL888" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AI143" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AM882" sqref="AM882"/>
+      <selection pane="bottomRight" activeCell="AJ158" sqref="AJ158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4619,7 +4619,7 @@
         <v>1102</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>272</v>
@@ -5618,7 +5618,7 @@
         <v>738</v>
       </c>
       <c r="AM32" s="5" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="AN32" s="5" t="s">
         <v>95</v>
@@ -6048,7 +6048,7 @@
         <v>1243</v>
       </c>
       <c r="AM45" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="AN45" s="5" t="s">
         <v>95</v>
@@ -6107,7 +6107,7 @@
         <v>1244</v>
       </c>
       <c r="AM46" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="AN46" s="5" t="s">
         <v>95</v>
@@ -7007,7 +7007,7 @@
         <v>727</v>
       </c>
       <c r="AM75" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="AN75" s="5" t="s">
         <v>1105</v>
@@ -7385,7 +7385,7 @@
         <v>100</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="AD89" s="13">
         <v>27.49</v>
@@ -7405,7 +7405,7 @@
         <v>100</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>95</v>
@@ -7423,7 +7423,7 @@
         <v>58</v>
       </c>
       <c r="AJ90" s="37" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="AK90" s="37" t="s">
         <v>870</v>
@@ -8788,7 +8788,7 @@
         <v>727</v>
       </c>
       <c r="AJ137" t="s">
-        <v>1245</v>
+        <v>1297</v>
       </c>
       <c r="AN137" s="5" t="s">
         <v>95</v>
@@ -8844,7 +8844,7 @@
         <v>727</v>
       </c>
       <c r="AJ138" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="AN138" s="5" t="s">
         <v>95</v>
@@ -8900,7 +8900,7 @@
         <v>727</v>
       </c>
       <c r="AJ139" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="AN139" s="5" t="s">
         <v>95</v>
@@ -8956,7 +8956,7 @@
         <v>727</v>
       </c>
       <c r="AJ140" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="AN140" s="5" t="s">
         <v>95</v>
@@ -9402,7 +9402,7 @@
         <v>727</v>
       </c>
       <c r="AJ155" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="AN155" s="5" t="s">
         <v>95</v>
@@ -9452,7 +9452,7 @@
         <v>727</v>
       </c>
       <c r="AJ156" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="AN156" s="5" t="s">
         <v>95</v>
@@ -9502,7 +9502,7 @@
         <v>727</v>
       </c>
       <c r="AJ157" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="AN157" s="5" t="s">
         <v>95</v>
@@ -9552,7 +9552,7 @@
         <v>727</v>
       </c>
       <c r="AJ158" t="s">
-        <v>1252</v>
+        <v>1298</v>
       </c>
       <c r="AN158" s="5" t="s">
         <v>95</v>
@@ -11283,7 +11283,7 @@
         <v>727</v>
       </c>
       <c r="AM211" s="5" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="AN211" s="5" t="s">
         <v>95</v>
@@ -11477,7 +11477,7 @@
         <v>805</v>
       </c>
       <c r="AJ217" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="AN217" s="5" t="s">
         <v>95</v>
@@ -11539,7 +11539,7 @@
         <v>805</v>
       </c>
       <c r="AJ218" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="AN218" s="5" t="s">
         <v>95</v>
@@ -11601,7 +11601,7 @@
         <v>805</v>
       </c>
       <c r="AJ219" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="AN219" s="5" t="s">
         <v>95</v>
@@ -11663,7 +11663,7 @@
         <v>805</v>
       </c>
       <c r="AJ220" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="AN220" s="5" t="s">
         <v>95</v>
@@ -11832,7 +11832,7 @@
         <v>727</v>
       </c>
       <c r="AM226" s="5" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="AN226" s="5" t="s">
         <v>95</v>
@@ -12025,7 +12025,7 @@
         <v>727</v>
       </c>
       <c r="AM233" s="5" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="AN233" s="5" t="s">
         <v>95</v>
@@ -12187,7 +12187,7 @@
         <v>728</v>
       </c>
       <c r="AM236" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="AN236" s="5" t="s">
         <v>95</v>
@@ -12794,7 +12794,7 @@
         <v>727</v>
       </c>
       <c r="AJ256" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="AN256" s="5" t="s">
         <v>1107</v>
@@ -12847,7 +12847,7 @@
         <v>727</v>
       </c>
       <c r="AJ257" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="AN257" s="5" t="s">
         <v>1107</v>
@@ -12900,7 +12900,7 @@
         <v>727</v>
       </c>
       <c r="AJ258" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="AN258" s="5" t="s">
         <v>1107</v>
@@ -12953,7 +12953,7 @@
         <v>727</v>
       </c>
       <c r="AJ259" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="AN259" s="5" t="s">
         <v>1107</v>
@@ -13922,7 +13922,7 @@
         <v>805</v>
       </c>
       <c r="AJ289" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="AN289" s="5" t="s">
         <v>95</v>
@@ -13984,7 +13984,7 @@
         <v>805</v>
       </c>
       <c r="AJ290" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="AN290" s="5" t="s">
         <v>95</v>
@@ -14046,7 +14046,7 @@
         <v>805</v>
       </c>
       <c r="AJ291" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="AN291" s="5" t="s">
         <v>95</v>
@@ -14069,7 +14069,7 @@
         <v>32</v>
       </c>
       <c r="E292" s="4" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="F292" s="4" t="s">
         <v>629</v>
@@ -14108,7 +14108,7 @@
         <v>805</v>
       </c>
       <c r="AJ292" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="AN292" s="5" t="s">
         <v>95</v>
@@ -17651,7 +17651,7 @@
         <v>1087</v>
       </c>
       <c r="AM402" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="AN402" s="5" t="s">
         <v>1098</v>
@@ -18398,7 +18398,7 @@
         <v>1087</v>
       </c>
       <c r="AM425" s="5" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="AN425" t="s">
         <v>1101</v>
@@ -19530,7 +19530,7 @@
         <v>1087</v>
       </c>
       <c r="AM457" s="5" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="AN457" t="s">
         <v>1101</v>
@@ -19673,7 +19673,7 @@
         <v>1087</v>
       </c>
       <c r="AM461" s="5" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="AN461" t="s">
         <v>1101</v>
@@ -19781,7 +19781,7 @@
         <v>1087</v>
       </c>
       <c r="AM464" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="AN464" s="5" t="s">
         <v>1101</v>
@@ -19819,7 +19819,7 @@
         <v>1087</v>
       </c>
       <c r="AM465" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="AN465" s="5" t="s">
         <v>1101</v>
@@ -21436,7 +21436,7 @@
         <v>400</v>
       </c>
       <c r="AM518" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="AN518" t="s">
         <v>1101</v>
@@ -21668,7 +21668,7 @@
         <v>1087</v>
       </c>
       <c r="AM523" s="5" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="AN523" s="5" t="s">
         <v>1101</v>
@@ -21961,7 +21961,7 @@
         <v>1087</v>
       </c>
       <c r="AM534" s="5" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="AN534" t="s">
         <v>1098</v>
@@ -22051,7 +22051,7 @@
         <v>1087</v>
       </c>
       <c r="AM537" s="5" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="AN537" s="5" t="s">
         <v>1098</v>
@@ -22891,7 +22891,7 @@
         <v>1087</v>
       </c>
       <c r="AM567" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="AN567" s="5" t="s">
         <v>1099</v>
@@ -22999,7 +22999,7 @@
         <v>1087</v>
       </c>
       <c r="AM570" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="AN570" s="5" t="s">
         <v>1100</v>
@@ -23646,7 +23646,7 @@
       </c>
       <c r="AD589" s="15"/>
       <c r="AJ589" s="5" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="AK589" s="5" t="s">
         <v>1049</v>
@@ -23747,7 +23747,7 @@
         <v>1087</v>
       </c>
       <c r="AM591" s="5" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="AN591" t="s">
         <v>1098</v>
@@ -26330,7 +26330,7 @@
         <v>1087</v>
       </c>
       <c r="AM659" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="AN659" t="s">
         <v>1098</v>
@@ -29290,7 +29290,7 @@
       </c>
       <c r="AD747" s="18"/>
       <c r="AM747" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="AN747" t="s">
         <v>1099</v>
@@ -29344,7 +29344,7 @@
       </c>
       <c r="AD748" s="18"/>
       <c r="AM748" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="AN748" t="s">
         <v>1099</v>
@@ -32105,7 +32105,7 @@
         <v>1087</v>
       </c>
       <c r="AM832" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="AN832" s="5" t="s">
         <v>1098</v>
@@ -32670,7 +32670,7 @@
         <v>1087</v>
       </c>
       <c r="AM848" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="AN848" s="5" t="s">
         <v>1099</v>
@@ -32749,7 +32749,7 @@
         <v>1087</v>
       </c>
       <c r="AM850" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="AN850" s="5" t="s">
         <v>1098</v>
@@ -33626,7 +33626,7 @@
         <v>1087</v>
       </c>
       <c r="AM876" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="AN876" t="s">
         <v>1099</v>
@@ -33819,7 +33819,7 @@
         <v>1087</v>
       </c>
       <c r="AM881" s="5" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="AN881" s="5" t="s">
         <v>1099</v>

</xml_diff>

<commit_message>
glintMask for 3043 retino 01
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DA8219-E214-3142-88BE-E0AC012625C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4DACBD-6B6F-B844-940F-242D74F08C18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="1160" windowWidth="24420" windowHeight="15060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="1160" windowWidth="25420" windowHeight="12040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eyeTrackingParams" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9832" uniqueCount="1299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9833" uniqueCount="1300">
   <si>
     <t>projectSubfolder</t>
   </si>
@@ -3927,6 +3927,9 @@
   </si>
   <si>
     <t>[4, 736, 1802, 2816, 5117, 6318, 8073, 9684, 11460, 12636, 13891, 15189, 16955, 18943]</t>
+  </si>
+  <si>
+    <t>[30 140 334 202]</t>
   </si>
 </sst>
 </file>
@@ -4466,10 +4469,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AI143" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E930" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ158" sqref="AJ158"/>
+      <selection pane="bottomRight" activeCell="E943" sqref="E943"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -35977,6 +35980,9 @@
       <c r="D942" s="4" t="s">
         <v>840</v>
       </c>
+      <c r="E942" s="4" t="s">
+        <v>1299</v>
+      </c>
       <c r="W942" s="5" t="s">
         <v>1240</v>
       </c>

</xml_diff>

<commit_message>
updated cameraTrans x0 vals
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4844C26-D1A2-DE40-8C95-53F91B26ADFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A1427B-8FB9-424A-8A7E-F3E36A9E9106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="460" windowWidth="23560" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2140" yWindow="460" windowWidth="23560" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eyeTrackingParams" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9851" uniqueCount="1318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9852" uniqueCount="1319">
   <si>
     <t>projectSubfolder</t>
   </si>
@@ -3905,9 +3905,6 @@
     <t>[-2.00; 1.34; 169.59]</t>
   </si>
   <si>
-    <t>[-0.24; -0.09; 165.71]</t>
-  </si>
-  <si>
     <t>[3.00; -1.67; 152.70]</t>
   </si>
   <si>
@@ -3941,9 +3938,6 @@
     <t>[2.16; -0.50; 178.96]</t>
   </si>
   <si>
-    <t>[1.88; -2.50; 178.98]</t>
-  </si>
-  <si>
     <t>[0.34; 0.50; 162.24]</t>
   </si>
   <si>
@@ -3984,6 +3978,15 @@
   </si>
   <si>
     <t>[0.48; -5.07; 159.71]</t>
+  </si>
+  <si>
+    <t>[-1.00; -0.99; 165.32]</t>
+  </si>
+  <si>
+    <t>[-1.50; 2.09; 156.10]</t>
+  </si>
+  <si>
+    <t>[1.88; -2.50; 178.96]</t>
   </si>
 </sst>
 </file>
@@ -4523,10 +4526,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AH525" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AG788" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ531" sqref="AJ531"/>
+      <selection pane="bottomRight" activeCell="AM802" sqref="AM802"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10156,7 +10159,7 @@
         <v>727</v>
       </c>
       <c r="AM174" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="AN174" s="5" t="s">
         <v>95</v>
@@ -10206,7 +10209,7 @@
         <v>727</v>
       </c>
       <c r="AM175" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="AN175" s="5" t="s">
         <v>95</v>
@@ -10791,7 +10794,7 @@
         <v>789</v>
       </c>
       <c r="AM192" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="AN192" s="5" t="s">
         <v>95</v>
@@ -13798,7 +13801,7 @@
         <v>727</v>
       </c>
       <c r="AM283" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="AN283" s="5" t="s">
         <v>95</v>
@@ -14118,7 +14121,7 @@
         <v>1252</v>
       </c>
       <c r="AM291" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="AN291" s="5" t="s">
         <v>95</v>
@@ -14183,7 +14186,7 @@
         <v>1253</v>
       </c>
       <c r="AM292" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="AN292" s="5" t="s">
         <v>95</v>
@@ -15593,7 +15596,7 @@
         <v>727</v>
       </c>
       <c r="AM334" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="AN334" s="5" t="s">
         <v>95</v>
@@ -15643,7 +15646,7 @@
         <v>727</v>
       </c>
       <c r="AM335" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="AN335" s="5" t="s">
         <v>95</v>
@@ -15693,7 +15696,7 @@
         <v>727</v>
       </c>
       <c r="AM336" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="AN336" s="5" t="s">
         <v>95</v>
@@ -15851,7 +15854,7 @@
         <v>727</v>
       </c>
       <c r="AM341" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="AN341" s="5" t="s">
         <v>95</v>
@@ -16067,7 +16070,7 @@
         <v>727</v>
       </c>
       <c r="AM348" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="AN348" s="5" t="s">
         <v>95</v>
@@ -16184,7 +16187,7 @@
         <v>727</v>
       </c>
       <c r="AM351" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="AN351" s="5" t="s">
         <v>95</v>
@@ -22960,7 +22963,7 @@
         <v>1079</v>
       </c>
       <c r="AM567" t="s">
-        <v>1291</v>
+        <v>1316</v>
       </c>
       <c r="AN567" s="5" t="s">
         <v>1091</v>
@@ -24449,7 +24452,7 @@
         <v>1079</v>
       </c>
       <c r="AM607" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="AN607" t="s">
         <v>1090</v>
@@ -24490,7 +24493,7 @@
         <v>1079</v>
       </c>
       <c r="AM608" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="AN608" t="s">
         <v>1090</v>
@@ -24607,7 +24610,7 @@
         <v>1079</v>
       </c>
       <c r="AM611" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="AN611" t="s">
         <v>1090</v>
@@ -25071,7 +25074,7 @@
         <v>1079</v>
       </c>
       <c r="AM625" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="AN625" t="s">
         <v>1091</v>
@@ -30013,7 +30016,7 @@
         <v>1079</v>
       </c>
       <c r="AM763" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="AN763" t="s">
         <v>1092</v>
@@ -30067,6 +30070,9 @@
       <c r="X765" s="5" t="s">
         <v>1079</v>
       </c>
+      <c r="AM765" t="s">
+        <v>1317</v>
+      </c>
       <c r="AN765" t="s">
         <v>1091</v>
       </c>
@@ -30224,7 +30230,7 @@
         <v>1079</v>
       </c>
       <c r="AM771" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="AN771" s="5" t="s">
         <v>1093</v>
@@ -30594,7 +30600,7 @@
         <v>1079</v>
       </c>
       <c r="AM782" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="AN782" t="s">
         <v>1093</v>
@@ -30981,7 +30987,7 @@
         <v>1079</v>
       </c>
       <c r="AM794" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="AN794" t="s">
         <v>1091</v>
@@ -31329,7 +31335,7 @@
         <v>1079</v>
       </c>
       <c r="AM803" t="s">
-        <v>1303</v>
+        <v>1318</v>
       </c>
       <c r="AN803" t="s">
         <v>1091</v>
@@ -34529,7 +34535,7 @@
         <v>1029</v>
       </c>
       <c r="AM895" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="AN895" s="5" t="s">
         <v>1092</v>
@@ -34837,7 +34843,7 @@
         <v>1079</v>
       </c>
       <c r="AM905" s="5" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="AN905" t="s">
         <v>1091</v>
@@ -36353,7 +36359,7 @@
         <v>1079</v>
       </c>
       <c r="AM953" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="AN953" t="s">
         <v>1090</v>
@@ -37192,7 +37198,7 @@
         <v>1079</v>
       </c>
       <c r="AM974" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="AN974" s="5" t="s">
         <v>1090</v>
@@ -37248,7 +37254,7 @@
         <v>1079</v>
       </c>
       <c r="AM975" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="AN975" s="5" t="s">
         <v>1090</v>

</xml_diff>

<commit_message>
Gaze cal source for 3045 sess 2
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A1427B-8FB9-424A-8A7E-F3E36A9E9106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B987E416-2743-924B-B1F1-4B87F58D5212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2140" yWindow="460" windowWidth="23560" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4526,10 +4526,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AG788" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AI956" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AM802" sqref="AM802"/>
+      <selection pane="bottomRight" activeCell="AM975" sqref="AM975"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -36868,7 +36868,7 @@
         <v>1079</v>
       </c>
       <c r="AN968" t="s">
-        <v>1090</v>
+        <v>1093</v>
       </c>
       <c r="AO968" t="s">
         <v>1059</v>
@@ -36921,7 +36921,7 @@
         <v>1079</v>
       </c>
       <c r="AN969" t="s">
-        <v>1090</v>
+        <v>1093</v>
       </c>
       <c r="AO969" t="s">
         <v>1059</v>
@@ -36986,7 +36986,7 @@
       <c r="AL970" s="4"/>
       <c r="AM970" s="4"/>
       <c r="AN970" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="AO970" t="s">
         <v>1059</v>
@@ -37039,7 +37039,7 @@
         <v>1079</v>
       </c>
       <c r="AN971" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="AO971" t="s">
         <v>1059</v>
@@ -37145,7 +37145,7 @@
         <v>1079</v>
       </c>
       <c r="AN973" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="AO973" t="s">
         <v>1059</v>
@@ -37200,8 +37200,8 @@
       <c r="AM974" t="s">
         <v>1312</v>
       </c>
-      <c r="AN974" s="5" t="s">
-        <v>1090</v>
+      <c r="AN974" t="s">
+        <v>1093</v>
       </c>
       <c r="AO974" t="s">
         <v>1059</v>
@@ -37256,8 +37256,8 @@
       <c r="AM975" t="s">
         <v>1313</v>
       </c>
-      <c r="AN975" s="5" t="s">
-        <v>1090</v>
+      <c r="AN975" t="s">
+        <v>1093</v>
       </c>
       <c r="AO975" t="s">
         <v>1059</v>
@@ -37309,8 +37309,8 @@
       <c r="X976" s="5" t="s">
         <v>1079</v>
       </c>
-      <c r="AN976" s="5" t="s">
-        <v>1092</v>
+      <c r="AN976" t="s">
+        <v>1093</v>
       </c>
       <c r="AO976" t="s">
         <v>1059</v>
@@ -37365,8 +37365,8 @@
       <c r="X977" s="5" t="s">
         <v>1079</v>
       </c>
-      <c r="AN977" s="5" t="s">
-        <v>1091</v>
+      <c r="AN977" t="s">
+        <v>1093</v>
       </c>
       <c r="AO977" t="s">
         <v>1059</v>

</xml_diff>

<commit_message>
Adjusting pupil range 3020 Movie 1
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B987E416-2743-924B-B1F1-4B87F58D5212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88DF2CC-CF21-794C-A9C2-81511CDBB172}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2140" yWindow="460" windowWidth="23560" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9852" uniqueCount="1319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9852" uniqueCount="1320">
   <si>
     <t>projectSubfolder</t>
   </si>
@@ -3987,6 +3987,9 @@
   </si>
   <si>
     <t>[1.88; -2.50; 178.96]</t>
+  </si>
+  <si>
+    <t>[53 150]</t>
   </si>
 </sst>
 </file>
@@ -4526,10 +4529,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AI956" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="J601" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AM975" sqref="AM975"/>
+      <selection pane="bottomRight" activeCell="K609" sqref="K609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -24481,7 +24484,7 @@
         <v>208</v>
       </c>
       <c r="K608" s="4" t="s">
-        <v>950</v>
+        <v>1319</v>
       </c>
       <c r="L608" s="4" t="s">
         <v>396</v>

</xml_diff>

<commit_message>
cameraTrans values for 3017 retino 01 and 3004 rest 04
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DA5980-6B45-3A49-A7AE-5B8353D6565F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AEA352-8766-534A-8283-93588AACDA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="460" windowWidth="23560" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="460" windowWidth="23560" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eyeTrackingParams" sheetId="1" r:id="rId1"/>
@@ -3890,9 +3890,6 @@
     <t>[30 140 334 202]</t>
   </si>
   <si>
-    <t>[-4.50; 1.03]</t>
-  </si>
-  <si>
     <t>[3.10; -2.54; 159.62]</t>
   </si>
   <si>
@@ -3977,9 +3974,6 @@
     <t>[0.48; -5.07; 159.71]</t>
   </si>
   <si>
-    <t>[-1.00; -0.99; 165.32]</t>
-  </si>
-  <si>
     <t>[-1.50; 2.09; 156.10]</t>
   </si>
   <si>
@@ -3990,6 +3984,12 @@
   </si>
   <si>
     <t>[ 0; pi]</t>
+  </si>
+  <si>
+    <t>[[-1.50; -0.72]</t>
+  </si>
+  <si>
+    <t>[-3.00; 0.03]</t>
   </si>
 </sst>
 </file>
@@ -4529,10 +4529,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="Q592" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AK15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S611" sqref="S611"/>
+      <selection pane="bottomRight" activeCell="AM32" sqref="AM32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5681,7 +5681,7 @@
         <v>738</v>
       </c>
       <c r="AM32" s="5" t="s">
-        <v>1286</v>
+        <v>1319</v>
       </c>
       <c r="AN32" s="5" t="s">
         <v>95</v>
@@ -6170,7 +6170,7 @@
         <v>1235</v>
       </c>
       <c r="AM46" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="AN46" s="5" t="s">
         <v>95</v>
@@ -10162,7 +10162,7 @@
         <v>727</v>
       </c>
       <c r="AM174" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="AN174" s="5" t="s">
         <v>95</v>
@@ -10212,7 +10212,7 @@
         <v>727</v>
       </c>
       <c r="AM175" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="AN175" s="5" t="s">
         <v>95</v>
@@ -10797,7 +10797,7 @@
         <v>789</v>
       </c>
       <c r="AM192" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="AN192" s="5" t="s">
         <v>95</v>
@@ -13804,7 +13804,7 @@
         <v>727</v>
       </c>
       <c r="AM283" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="AN283" s="5" t="s">
         <v>95</v>
@@ -14124,7 +14124,7 @@
         <v>1251</v>
       </c>
       <c r="AM291" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="AN291" s="5" t="s">
         <v>95</v>
@@ -14189,7 +14189,7 @@
         <v>1252</v>
       </c>
       <c r="AM292" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="AN292" s="5" t="s">
         <v>95</v>
@@ -15599,7 +15599,7 @@
         <v>727</v>
       </c>
       <c r="AM334" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="AN334" s="5" t="s">
         <v>95</v>
@@ -15649,7 +15649,7 @@
         <v>727</v>
       </c>
       <c r="AM335" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="AN335" s="5" t="s">
         <v>95</v>
@@ -15699,7 +15699,7 @@
         <v>727</v>
       </c>
       <c r="AM336" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="AN336" s="5" t="s">
         <v>95</v>
@@ -15857,7 +15857,7 @@
         <v>727</v>
       </c>
       <c r="AM341" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="AN341" s="5" t="s">
         <v>95</v>
@@ -16073,7 +16073,7 @@
         <v>727</v>
       </c>
       <c r="AM348" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="AN348" s="5" t="s">
         <v>95</v>
@@ -16190,7 +16190,7 @@
         <v>727</v>
       </c>
       <c r="AM351" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="AN351" s="5" t="s">
         <v>95</v>
@@ -19605,7 +19605,7 @@
         <v>1078</v>
       </c>
       <c r="AM457" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="AN457" t="s">
         <v>1092</v>
@@ -22036,7 +22036,7 @@
         <v>1078</v>
       </c>
       <c r="AM534" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="AN534" t="s">
         <v>1089</v>
@@ -22966,7 +22966,7 @@
         <v>1078</v>
       </c>
       <c r="AM567" t="s">
-        <v>1315</v>
+        <v>1318</v>
       </c>
       <c r="AN567" s="5" t="s">
         <v>1090</v>
@@ -24405,13 +24405,13 @@
         <v>208</v>
       </c>
       <c r="K606" s="4" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="L606" s="4" t="s">
         <v>396</v>
       </c>
       <c r="T606" s="4" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="U606" s="4" t="s">
         <v>690</v>
@@ -24449,13 +24449,13 @@
         <v>208</v>
       </c>
       <c r="K607" s="4" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="L607" s="4" t="s">
         <v>396</v>
       </c>
       <c r="T607" s="4" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="U607" s="4" t="s">
         <v>690</v>
@@ -24467,7 +24467,7 @@
         <v>1078</v>
       </c>
       <c r="AM607" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="AN607" t="s">
         <v>1089</v>
@@ -24496,13 +24496,13 @@
         <v>208</v>
       </c>
       <c r="K608" s="4" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="L608" s="4" t="s">
         <v>396</v>
       </c>
       <c r="T608" s="4" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="U608" s="4" t="s">
         <v>690</v>
@@ -24514,7 +24514,7 @@
         <v>1078</v>
       </c>
       <c r="AM608" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="AN608" t="s">
         <v>1089</v>
@@ -24543,13 +24543,13 @@
         <v>208</v>
       </c>
       <c r="K609" s="4" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="L609" s="4" t="s">
         <v>396</v>
       </c>
       <c r="T609" s="4" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="U609" s="4" t="s">
         <v>690</v>
@@ -24587,13 +24587,13 @@
         <v>208</v>
       </c>
       <c r="K610" s="4" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="L610" s="4" t="s">
         <v>396</v>
       </c>
       <c r="T610" s="4" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="U610" s="4" t="s">
         <v>690</v>
@@ -24631,13 +24631,13 @@
         <v>208</v>
       </c>
       <c r="K611" s="4" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="L611" s="4" t="s">
         <v>396</v>
       </c>
       <c r="T611" s="4" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="U611" s="4" t="s">
         <v>690</v>
@@ -24649,7 +24649,7 @@
         <v>1078</v>
       </c>
       <c r="AM611" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="AN611" t="s">
         <v>1089</v>
@@ -24678,13 +24678,13 @@
         <v>208</v>
       </c>
       <c r="K612" s="4" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="L612" s="4" t="s">
         <v>396</v>
       </c>
       <c r="T612" s="4" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="U612" s="4" t="s">
         <v>690</v>
@@ -24722,13 +24722,13 @@
         <v>208</v>
       </c>
       <c r="K613" s="4" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="L613" s="4" t="s">
         <v>396</v>
       </c>
       <c r="T613" s="4" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="U613" s="4" t="s">
         <v>690</v>
@@ -24766,13 +24766,13 @@
         <v>208</v>
       </c>
       <c r="K614" s="4" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="L614" s="4" t="s">
         <v>396</v>
       </c>
       <c r="T614" s="4" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="U614" s="4" t="s">
         <v>690</v>
@@ -24810,13 +24810,13 @@
         <v>208</v>
       </c>
       <c r="K615" s="4" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="L615" s="4" t="s">
         <v>396</v>
       </c>
       <c r="T615" s="4" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="U615" s="4" t="s">
         <v>690</v>
@@ -25137,7 +25137,7 @@
         <v>1078</v>
       </c>
       <c r="AM625" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="AN625" t="s">
         <v>1090</v>
@@ -30079,7 +30079,7 @@
         <v>1078</v>
       </c>
       <c r="AM763" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="AN763" t="s">
         <v>1091</v>
@@ -30134,7 +30134,7 @@
         <v>1078</v>
       </c>
       <c r="AM765" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="AN765" t="s">
         <v>1090</v>
@@ -30293,7 +30293,7 @@
         <v>1078</v>
       </c>
       <c r="AM771" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="AN771" s="5" t="s">
         <v>1092</v>
@@ -30663,7 +30663,7 @@
         <v>1078</v>
       </c>
       <c r="AM782" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="AN782" t="s">
         <v>1092</v>
@@ -31050,7 +31050,7 @@
         <v>1078</v>
       </c>
       <c r="AM794" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="AN794" t="s">
         <v>1090</v>
@@ -31398,7 +31398,7 @@
         <v>1078</v>
       </c>
       <c r="AM803" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="AN803" t="s">
         <v>1090</v>
@@ -34598,7 +34598,7 @@
         <v>1028</v>
       </c>
       <c r="AM895" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="AN895" s="5" t="s">
         <v>1091</v>
@@ -34906,7 +34906,7 @@
         <v>1078</v>
       </c>
       <c r="AM905" s="5" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="AN905" t="s">
         <v>1090</v>
@@ -36422,7 +36422,7 @@
         <v>1078</v>
       </c>
       <c r="AM953" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="AN953" t="s">
         <v>1089</v>
@@ -37261,7 +37261,7 @@
         <v>1078</v>
       </c>
       <c r="AM974" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="AN974" t="s">
         <v>1092</v>
@@ -37317,7 +37317,7 @@
         <v>1078</v>
       </c>
       <c r="AM975" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="AN975" t="s">
         <v>1092</v>

</xml_diff>

<commit_message>
3037 sess 2, avoid the crummy gaze cal
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6199A3-B795-4842-AB10-4C121B966365}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8998D8-6BFE-334F-AD5D-46BC1FE93265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="460" windowWidth="23560" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4529,10 +4529,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AK65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AK849" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AN74" sqref="AN74"/>
+      <selection pane="bottomRight" activeCell="AM864" sqref="AM864"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -33278,7 +33278,7 @@
         <v>1078</v>
       </c>
       <c r="AN861" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="AO861" t="s">
         <v>1058</v>
@@ -33430,7 +33430,7 @@
         <v>1078</v>
       </c>
       <c r="AN865" s="5" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="AO865" t="s">
         <v>1058</v>
@@ -33468,7 +33468,7 @@
         <v>1078</v>
       </c>
       <c r="AN866" s="5" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="AO866" t="s">
         <v>1058</v>

</xml_diff>

<commit_message>
3105 retino runs 2, 4, custom frame set
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C02600-3671-254B-912F-84FEB76545DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF680EF-A8D9-8D49-9600-EAAD7A8E6868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="460" windowWidth="23560" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="460" windowWidth="20480" windowHeight="16400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eyeTrackingParams" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9872" uniqueCount="1319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9874" uniqueCount="1321">
   <si>
     <t>projectSubfolder</t>
   </si>
@@ -3987,6 +3987,12 @@
   </si>
   <si>
     <t>[-50,-40,0,1.0]</t>
+  </si>
+  <si>
+    <t>[190, 4433, 6016, 8052, 3116, 1043, 11239, 8459, 18569, 10082, 5736, 17712, 15517, 13053, 16975, 8672, 20494, 6570, 8720, 6506, 6340]</t>
+  </si>
+  <si>
+    <t>[399, 14251, 14927, 11684, 18776, 12762, 10711,  7343,  7007, 20598, 18147,  8631,  3789,  5350,  2777, 13778, 14380]</t>
   </si>
 </sst>
 </file>
@@ -4526,10 +4532,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="T213" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AI516" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X17" sqref="X17"/>
+      <selection pane="bottomRight" activeCell="AJ540" sqref="AJ540"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -22122,6 +22128,9 @@
       <c r="X537" s="5" t="s">
         <v>1071</v>
       </c>
+      <c r="AJ537" s="5" t="s">
+        <v>1319</v>
+      </c>
       <c r="AM537" s="5" t="s">
         <v>1265</v>
       </c>
@@ -22182,6 +22191,9 @@
       </c>
       <c r="X539" s="5" t="s">
         <v>1071</v>
+      </c>
+      <c r="AJ539" s="5" t="s">
+        <v>1320</v>
       </c>
       <c r="AN539" s="5" t="s">
         <v>1085</v>

</xml_diff>

<commit_message>
Custom frame set for 3031 rest 4
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB01E4C-D385-CD4B-9861-286091D64AD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1102C073-0BD7-D340-8489-FB7656E889C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="460" windowWidth="20480" windowHeight="16400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="460" windowWidth="27220" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eyeTrackingParams" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9874" uniqueCount="1321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9875" uniqueCount="1322">
   <si>
     <t>projectSubfolder</t>
   </si>
@@ -3993,6 +3993,9 @@
   </si>
   <si>
     <t>[-1.50; -0.72]</t>
+  </si>
+  <si>
+    <t>[15201, 2530, 3373, 5147, 6696, 9116, 10332, 11972, 12069, 13618, 15206, 16788, 19183, 20235, 11978, 20249, 20255, 11666, 10434, 5196, 20143, 15049, 10157]</t>
   </si>
 </sst>
 </file>
@@ -4002,7 +4005,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4097,6 +4100,12 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -4126,7 +4135,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4181,6 +4190,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4532,10 +4542,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AJ549" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AG237" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AM568" sqref="AM568"/>
+      <selection pane="bottomRight" activeCell="AJ245" sqref="AJ245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12557,6 +12567,9 @@
       <c r="X244" s="5" t="s">
         <v>1316</v>
       </c>
+      <c r="AJ244" s="38" t="s">
+        <v>1321</v>
+      </c>
       <c r="AN244" s="5" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
Using gazeCal 03 for 3045
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/code/eyeTrackingParams.xlsx
+++ b/code/eyeTrackingParams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aguirre/Documents/MATLAB/projects/eyeTrackTOMEAnalysis/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF60E36-8C72-5A41-91CF-89ADBCDEEA88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901147C3-BFC6-D946-AF66-F73BC1496DCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="460" windowWidth="27220" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="460" windowWidth="25720" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eyeTrackingParams" sheetId="1" r:id="rId1"/>
@@ -4542,10 +4542,10 @@
   <dimension ref="A1:AQ979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AG237" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AK958" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ244" sqref="AJ244"/>
+      <selection pane="bottomRight" activeCell="AN977" sqref="AN977"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -36953,7 +36953,7 @@
         <v>1071</v>
       </c>
       <c r="AN968" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AO968" t="s">
         <v>1051</v>
@@ -37006,7 +37006,7 @@
         <v>1071</v>
       </c>
       <c r="AN969" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AO969" t="s">
         <v>1051</v>
@@ -37071,7 +37071,7 @@
       <c r="AL970" s="4"/>
       <c r="AM970" s="4"/>
       <c r="AN970" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AO970" t="s">
         <v>1051</v>
@@ -37124,7 +37124,7 @@
         <v>1071</v>
       </c>
       <c r="AN971" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AO971" t="s">
         <v>1051</v>
@@ -37177,7 +37177,7 @@
         <v>1071</v>
       </c>
       <c r="AN972" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AO972" t="s">
         <v>1051</v>
@@ -37230,7 +37230,7 @@
         <v>1071</v>
       </c>
       <c r="AN973" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AO973" t="s">
         <v>1051</v>
@@ -37286,7 +37286,7 @@
         <v>1302</v>
       </c>
       <c r="AN974" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AO974" t="s">
         <v>1051</v>
@@ -37342,7 +37342,7 @@
         <v>1303</v>
       </c>
       <c r="AN975" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AO975" t="s">
         <v>1051</v>
@@ -37395,7 +37395,7 @@
         <v>1071</v>
       </c>
       <c r="AN976" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AO976" t="s">
         <v>1051</v>
@@ -37451,7 +37451,7 @@
         <v>1071</v>
       </c>
       <c r="AN977" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="AO977" t="s">
         <v>1051</v>

</xml_diff>